<commit_message>
no early investment - both models
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_opmode_UC.xlsx
+++ b/SuppXLS/Scen_opmode_UC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\OSeMOSYS_EUWest\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1235C59D-CD37-4C53-AF07-AB6B33354198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D0906-D93D-42E0-B742-80F1A3029F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="130">
   <si>
     <t>process</t>
   </si>
@@ -62,9 +62,6 @@
     <t>attribute</t>
   </si>
   <si>
-    <t>NCAP_PKCNT</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -74,13 +71,7 @@
     <t>commodity</t>
   </si>
   <si>
-    <t>ELC*</t>
-  </si>
-  <si>
     <t>top_check</t>
-  </si>
-  <si>
-    <t>out</t>
   </si>
   <si>
     <t>year</t>
@@ -419,12 +410,6 @@
     <t>PWRURNPRTXX01</t>
   </si>
   <si>
-    <t>INVCOST</t>
-  </si>
-  <si>
-    <t>om2*</t>
-  </si>
-  <si>
     <t>START</t>
   </si>
   <si>
@@ -437,16 +422,7 @@
     <t>PWR*</t>
   </si>
   <si>
-    <t>AFA</t>
-  </si>
-  <si>
     <t>limtype</t>
-  </si>
-  <si>
-    <t>LO</t>
-  </si>
-  <si>
-    <t>PWRCCG*</t>
   </si>
 </sst>
 </file>
@@ -826,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BE114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AW8" sqref="AW8:BE8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -860,7 +836,7 @@
         <v>6</v>
       </c>
       <c r="AW3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:57" x14ac:dyDescent="0.5">
@@ -1000,30 +976,30 @@
         <v>0</v>
       </c>
       <c r="AY4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AZ4" t="s">
+        <v>11</v>
+      </c>
+      <c r="BA4" t="s">
         <v>12</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BB4" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC4" t="s">
         <v>14</v>
       </c>
-      <c r="BB4" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>17</v>
-      </c>
       <c r="BD4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="BE4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>0.9</v>
@@ -1142,7 +1118,7 @@
         <v>op mode_PWRCCGAUTXX00</v>
       </c>
       <c r="AQ5" t="str">
-        <f>C5&amp;"*"</f>
+        <f t="shared" ref="AQ5:AQ36" si="1">C5&amp;"*"</f>
         <v>PWRCCGAUTXX00*</v>
       </c>
       <c r="AR5" s="1">
@@ -1156,30 +1132,21 @@
         <v>3</v>
       </c>
       <c r="AW5" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="AX5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AY5">
-        <v>0</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>13</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB5">
-        <v>2020</v>
-      </c>
-      <c r="BC5">
-        <v>1</v>
+        <v>2025</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>0.9</v>
@@ -1294,15 +1261,15 @@
         <v>op mode_PWRCCGAUTXX01</v>
       </c>
       <c r="AP6" t="str">
-        <f t="shared" ref="AP6:AP69" si="1">AN6</f>
+        <f t="shared" ref="AP6:AP69" si="2">AN6</f>
         <v>op mode_PWRCCGAUTXX01</v>
       </c>
       <c r="AQ6" t="str">
-        <f>C6&amp;"*"</f>
+        <f t="shared" si="1"/>
         <v>PWRCCGAUTXX01*</v>
       </c>
       <c r="AR6" s="1">
-        <f t="shared" ref="AR6:AR69" si="2">-1/31.536</f>
+        <f t="shared" ref="AR6:AR69" si="3">-1/31.536</f>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS6">
@@ -1310,20 +1277,11 @@
       </c>
       <c r="AT6">
         <v>3</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>128</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>129</v>
-      </c>
-      <c r="AY6">
-        <v>1E-3</v>
       </c>
     </row>
     <row r="7" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>0.9</v>
@@ -1438,15 +1396,15 @@
         <v>op mode_PWRCCGBELXX00</v>
       </c>
       <c r="AP7" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGBELXX00</v>
+      </c>
+      <c r="AQ7" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGBELXX00</v>
-      </c>
-      <c r="AQ7" t="str">
-        <f>C7&amp;"*"</f>
         <v>PWRCCGBELXX00*</v>
       </c>
       <c r="AR7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS7">
@@ -1454,23 +1412,11 @@
       </c>
       <c r="AT7">
         <v>3</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>133</v>
-      </c>
-      <c r="AY7">
-        <v>2025</v>
-      </c>
-      <c r="BD7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>0.9</v>
@@ -1585,15 +1531,15 @@
         <v>op mode_PWRCCGBELXX01</v>
       </c>
       <c r="AP8" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGBELXX01</v>
+      </c>
+      <c r="AQ8" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGBELXX01</v>
-      </c>
-      <c r="AQ8" t="str">
-        <f>C8&amp;"*"</f>
         <v>PWRCCGBELXX01*</v>
       </c>
       <c r="AR8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS8">
@@ -1605,7 +1551,7 @@
     </row>
     <row r="9" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>0.9</v>
@@ -1720,15 +1666,15 @@
         <v>op mode_PWRCCGCHEXX00</v>
       </c>
       <c r="AP9" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGCHEXX00</v>
+      </c>
+      <c r="AQ9" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGCHEXX00</v>
-      </c>
-      <c r="AQ9" t="str">
-        <f>C9&amp;"*"</f>
         <v>PWRCCGCHEXX00*</v>
       </c>
       <c r="AR9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS9">
@@ -1740,7 +1686,7 @@
     </row>
     <row r="10" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>0.9</v>
@@ -1855,15 +1801,15 @@
         <v>op mode_PWRCCGCHEXX01</v>
       </c>
       <c r="AP10" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGCHEXX01</v>
+      </c>
+      <c r="AQ10" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGCHEXX01</v>
-      </c>
-      <c r="AQ10" t="str">
-        <f>C10&amp;"*"</f>
         <v>PWRCCGCHEXX01*</v>
       </c>
       <c r="AR10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS10">
@@ -1871,26 +1817,11 @@
       </c>
       <c r="AT10">
         <v>3</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>134</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>137</v>
-      </c>
-      <c r="AY10">
-        <v>0.3</v>
-      </c>
-      <c r="BB10">
-        <v>2025</v>
-      </c>
-      <c r="BE10" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="11" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>0.9</v>
@@ -2005,15 +1936,15 @@
         <v>op mode_PWRCCGDEUXX00</v>
       </c>
       <c r="AP11" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGDEUXX00</v>
+      </c>
+      <c r="AQ11" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGDEUXX00</v>
-      </c>
-      <c r="AQ11" t="str">
-        <f>C11&amp;"*"</f>
         <v>PWRCCGDEUXX00*</v>
       </c>
       <c r="AR11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS11">
@@ -2021,27 +1952,11 @@
       </c>
       <c r="AT11">
         <v>3</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>134</v>
-      </c>
-      <c r="AX11" t="str">
-        <f>AX10</f>
-        <v>PWRCCG*</v>
-      </c>
-      <c r="AY11">
-        <v>5</v>
-      </c>
-      <c r="BB11">
-        <v>0</v>
-      </c>
-      <c r="BE11" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>0.9</v>
@@ -2156,15 +2071,15 @@
         <v>op mode_PWRCCGDEUXX01</v>
       </c>
       <c r="AP12" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGDEUXX01</v>
+      </c>
+      <c r="AQ12" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGDEUXX01</v>
-      </c>
-      <c r="AQ12" t="str">
-        <f>C12&amp;"*"</f>
         <v>PWRCCGDEUXX01*</v>
       </c>
       <c r="AR12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS12">
@@ -2176,7 +2091,7 @@
     </row>
     <row r="13" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>0.9</v>
@@ -2291,15 +2206,15 @@
         <v>op mode_PWRCCGESPXX00</v>
       </c>
       <c r="AP13" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGESPXX00</v>
+      </c>
+      <c r="AQ13" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGESPXX00</v>
-      </c>
-      <c r="AQ13" t="str">
-        <f>C13&amp;"*"</f>
         <v>PWRCCGESPXX00*</v>
       </c>
       <c r="AR13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS13">
@@ -2311,7 +2226,7 @@
     </row>
     <row r="14" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>0.9</v>
@@ -2426,15 +2341,15 @@
         <v>op mode_PWRCCGESPXX01</v>
       </c>
       <c r="AP14" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGESPXX01</v>
+      </c>
+      <c r="AQ14" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGESPXX01</v>
-      </c>
-      <c r="AQ14" t="str">
-        <f>C14&amp;"*"</f>
         <v>PWRCCGESPXX01*</v>
       </c>
       <c r="AR14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS14">
@@ -2446,7 +2361,7 @@
     </row>
     <row r="15" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D15">
         <v>0.9</v>
@@ -2561,15 +2476,15 @@
         <v>op mode_PWRCCGFRAXX00</v>
       </c>
       <c r="AP15" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGFRAXX00</v>
+      </c>
+      <c r="AQ15" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGFRAXX00</v>
-      </c>
-      <c r="AQ15" t="str">
-        <f>C15&amp;"*"</f>
         <v>PWRCCGFRAXX00*</v>
       </c>
       <c r="AR15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS15">
@@ -2581,7 +2496,7 @@
     </row>
     <row r="16" spans="2:57" x14ac:dyDescent="0.5">
       <c r="C16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16">
         <v>0.9</v>
@@ -2696,15 +2611,15 @@
         <v>op mode_PWRCCGFRAXX01</v>
       </c>
       <c r="AP16" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGFRAXX01</v>
+      </c>
+      <c r="AQ16" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGFRAXX01</v>
-      </c>
-      <c r="AQ16" t="str">
-        <f>C16&amp;"*"</f>
         <v>PWRCCGFRAXX01*</v>
       </c>
       <c r="AR16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS16">
@@ -2716,7 +2631,7 @@
     </row>
     <row r="17" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17">
         <v>0.9</v>
@@ -2831,15 +2746,15 @@
         <v>op mode_PWRCCGITAXX00</v>
       </c>
       <c r="AP17" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGITAXX00</v>
+      </c>
+      <c r="AQ17" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGITAXX00</v>
-      </c>
-      <c r="AQ17" t="str">
-        <f>C17&amp;"*"</f>
         <v>PWRCCGITAXX00*</v>
       </c>
       <c r="AR17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS17">
@@ -2851,7 +2766,7 @@
     </row>
     <row r="18" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D18">
         <v>0.9</v>
@@ -2966,15 +2881,15 @@
         <v>op mode_PWRCCGITAXX01</v>
       </c>
       <c r="AP18" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGITAXX01</v>
+      </c>
+      <c r="AQ18" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGITAXX01</v>
-      </c>
-      <c r="AQ18" t="str">
-        <f>C18&amp;"*"</f>
         <v>PWRCCGITAXX01*</v>
       </c>
       <c r="AR18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS18">
@@ -2986,7 +2901,7 @@
     </row>
     <row r="19" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D19">
         <v>0.9</v>
@@ -3101,15 +3016,15 @@
         <v>op mode_PWRCCGLUXXX00</v>
       </c>
       <c r="AP19" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGLUXXX00</v>
+      </c>
+      <c r="AQ19" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGLUXXX00</v>
-      </c>
-      <c r="AQ19" t="str">
-        <f>C19&amp;"*"</f>
         <v>PWRCCGLUXXX00*</v>
       </c>
       <c r="AR19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS19">
@@ -3121,7 +3036,7 @@
     </row>
     <row r="20" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D20">
         <v>0.9</v>
@@ -3236,15 +3151,15 @@
         <v>op mode_PWRCCGLUXXX01</v>
       </c>
       <c r="AP20" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGLUXXX01</v>
+      </c>
+      <c r="AQ20" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGLUXXX01</v>
-      </c>
-      <c r="AQ20" t="str">
-        <f>C20&amp;"*"</f>
         <v>PWRCCGLUXXX01*</v>
       </c>
       <c r="AR20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS20">
@@ -3256,7 +3171,7 @@
     </row>
     <row r="21" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D21">
         <v>0.9</v>
@@ -3371,15 +3286,15 @@
         <v>op mode_PWRCCGNLDXX00</v>
       </c>
       <c r="AP21" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGNLDXX00</v>
+      </c>
+      <c r="AQ21" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGNLDXX00</v>
-      </c>
-      <c r="AQ21" t="str">
-        <f>C21&amp;"*"</f>
         <v>PWRCCGNLDXX00*</v>
       </c>
       <c r="AR21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS21">
@@ -3391,7 +3306,7 @@
     </row>
     <row r="22" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D22">
         <v>0.9</v>
@@ -3506,15 +3421,15 @@
         <v>op mode_PWRCCGNLDXX01</v>
       </c>
       <c r="AP22" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGNLDXX01</v>
+      </c>
+      <c r="AQ22" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGNLDXX01</v>
-      </c>
-      <c r="AQ22" t="str">
-        <f>C22&amp;"*"</f>
         <v>PWRCCGNLDXX01*</v>
       </c>
       <c r="AR22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS22">
@@ -3526,7 +3441,7 @@
     </row>
     <row r="23" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D23">
         <v>0.9</v>
@@ -3641,15 +3556,15 @@
         <v>op mode_PWRCCGPRTXX00</v>
       </c>
       <c r="AP23" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGPRTXX00</v>
+      </c>
+      <c r="AQ23" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGPRTXX00</v>
-      </c>
-      <c r="AQ23" t="str">
-        <f>C23&amp;"*"</f>
         <v>PWRCCGPRTXX00*</v>
       </c>
       <c r="AR23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS23">
@@ -3661,7 +3576,7 @@
     </row>
     <row r="24" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D24">
         <v>0.9</v>
@@ -3776,15 +3691,15 @@
         <v>op mode_PWRCCGPRTXX01</v>
       </c>
       <c r="AP24" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCGPRTXX01</v>
+      </c>
+      <c r="AQ24" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCGPRTXX01</v>
-      </c>
-      <c r="AQ24" t="str">
-        <f>C24&amp;"*"</f>
         <v>PWRCCGPRTXX01*</v>
       </c>
       <c r="AR24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS24">
@@ -3796,7 +3711,7 @@
     </row>
     <row r="25" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D25">
         <v>0.9</v>
@@ -3911,15 +3826,15 @@
         <v>op mode_PWRCCSAUTXX01</v>
       </c>
       <c r="AP25" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSAUTXX01</v>
+      </c>
+      <c r="AQ25" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSAUTXX01</v>
-      </c>
-      <c r="AQ25" t="str">
-        <f>C25&amp;"*"</f>
         <v>PWRCCSAUTXX01*</v>
       </c>
       <c r="AR25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS25">
@@ -3931,7 +3846,7 @@
     </row>
     <row r="26" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D26">
         <v>0.9</v>
@@ -4046,15 +3961,15 @@
         <v>op mode_PWRCCSBELXX01</v>
       </c>
       <c r="AP26" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSBELXX01</v>
+      </c>
+      <c r="AQ26" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSBELXX01</v>
-      </c>
-      <c r="AQ26" t="str">
-        <f>C26&amp;"*"</f>
         <v>PWRCCSBELXX01*</v>
       </c>
       <c r="AR26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS26">
@@ -4066,7 +3981,7 @@
     </row>
     <row r="27" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D27">
         <v>0.9</v>
@@ -4181,15 +4096,15 @@
         <v>op mode_PWRCCSCHEXX01</v>
       </c>
       <c r="AP27" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSCHEXX01</v>
+      </c>
+      <c r="AQ27" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSCHEXX01</v>
-      </c>
-      <c r="AQ27" t="str">
-        <f>C27&amp;"*"</f>
         <v>PWRCCSCHEXX01*</v>
       </c>
       <c r="AR27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS27">
@@ -4201,7 +4116,7 @@
     </row>
     <row r="28" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D28">
         <v>0.9</v>
@@ -4316,15 +4231,15 @@
         <v>op mode_PWRCCSDEUXX01</v>
       </c>
       <c r="AP28" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSDEUXX01</v>
+      </c>
+      <c r="AQ28" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSDEUXX01</v>
-      </c>
-      <c r="AQ28" t="str">
-        <f>C28&amp;"*"</f>
         <v>PWRCCSDEUXX01*</v>
       </c>
       <c r="AR28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS28">
@@ -4336,7 +4251,7 @@
     </row>
     <row r="29" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D29">
         <v>0.9</v>
@@ -4451,15 +4366,15 @@
         <v>op mode_PWRCCSESPXX01</v>
       </c>
       <c r="AP29" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSESPXX01</v>
+      </c>
+      <c r="AQ29" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSESPXX01</v>
-      </c>
-      <c r="AQ29" t="str">
-        <f>C29&amp;"*"</f>
         <v>PWRCCSESPXX01*</v>
       </c>
       <c r="AR29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS29">
@@ -4471,7 +4386,7 @@
     </row>
     <row r="30" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D30">
         <v>0.9</v>
@@ -4586,15 +4501,15 @@
         <v>op mode_PWRCCSFRAXX01</v>
       </c>
       <c r="AP30" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSFRAXX01</v>
+      </c>
+      <c r="AQ30" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSFRAXX01</v>
-      </c>
-      <c r="AQ30" t="str">
-        <f>C30&amp;"*"</f>
         <v>PWRCCSFRAXX01*</v>
       </c>
       <c r="AR30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS30">
@@ -4606,7 +4521,7 @@
     </row>
     <row r="31" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C31" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D31">
         <v>0.9</v>
@@ -4721,15 +4636,15 @@
         <v>op mode_PWRCCSITAXX01</v>
       </c>
       <c r="AP31" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSITAXX01</v>
+      </c>
+      <c r="AQ31" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSITAXX01</v>
-      </c>
-      <c r="AQ31" t="str">
-        <f>C31&amp;"*"</f>
         <v>PWRCCSITAXX01*</v>
       </c>
       <c r="AR31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS31">
@@ -4741,7 +4656,7 @@
     </row>
     <row r="32" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D32">
         <v>0.9</v>
@@ -4856,15 +4771,15 @@
         <v>op mode_PWRCCSLUXXX01</v>
       </c>
       <c r="AP32" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSLUXXX01</v>
+      </c>
+      <c r="AQ32" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSLUXXX01</v>
-      </c>
-      <c r="AQ32" t="str">
-        <f>C32&amp;"*"</f>
         <v>PWRCCSLUXXX01*</v>
       </c>
       <c r="AR32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS32">
@@ -4876,7 +4791,7 @@
     </row>
     <row r="33" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D33">
         <v>0.9</v>
@@ -4991,15 +4906,15 @@
         <v>op mode_PWRCCSNLDXX01</v>
       </c>
       <c r="AP33" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSNLDXX01</v>
+      </c>
+      <c r="AQ33" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSNLDXX01</v>
-      </c>
-      <c r="AQ33" t="str">
-        <f>C33&amp;"*"</f>
         <v>PWRCCSNLDXX01*</v>
       </c>
       <c r="AR33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS33">
@@ -5011,7 +4926,7 @@
     </row>
     <row r="34" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D34">
         <v>0.9</v>
@@ -5126,15 +5041,15 @@
         <v>op mode_PWRCCSPRTXX01</v>
       </c>
       <c r="AP34" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCCSPRTXX01</v>
+      </c>
+      <c r="AQ34" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCCSPRTXX01</v>
-      </c>
-      <c r="AQ34" t="str">
-        <f>C34&amp;"*"</f>
         <v>PWRCCSPRTXX01*</v>
       </c>
       <c r="AR34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS34">
@@ -5146,7 +5061,7 @@
     </row>
     <row r="35" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C35" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D35">
         <v>0.9</v>
@@ -5261,15 +5176,15 @@
         <v>op mode_PWRCOAAUTXX01</v>
       </c>
       <c r="AP35" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOAAUTXX01</v>
+      </c>
+      <c r="AQ35" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCOAAUTXX01</v>
-      </c>
-      <c r="AQ35" t="str">
-        <f>C35&amp;"*"</f>
         <v>PWRCOAAUTXX01*</v>
       </c>
       <c r="AR35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS35">
@@ -5281,7 +5196,7 @@
     </row>
     <row r="36" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C36" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D36">
         <v>0.9</v>
@@ -5396,15 +5311,15 @@
         <v>op mode_PWRCOABELXX01</v>
       </c>
       <c r="AP36" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOABELXX01</v>
+      </c>
+      <c r="AQ36" t="str">
         <f t="shared" si="1"/>
-        <v>op mode_PWRCOABELXX01</v>
-      </c>
-      <c r="AQ36" t="str">
-        <f>C36&amp;"*"</f>
         <v>PWRCOABELXX01*</v>
       </c>
       <c r="AR36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS36">
@@ -5416,7 +5331,7 @@
     </row>
     <row r="37" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C37" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D37">
         <v>0.9</v>
@@ -5527,19 +5442,19 @@
         <v>0.9</v>
       </c>
       <c r="AN37" t="str">
-        <f t="shared" ref="AN37:AN70" si="3">"op mode_"&amp;LEFT(AQ37,LEN(AQ37)-1)</f>
+        <f t="shared" ref="AN37:AN70" si="4">"op mode_"&amp;LEFT(AQ37,LEN(AQ37)-1)</f>
         <v>op mode_PWRCOACHEXX01</v>
       </c>
       <c r="AP37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>op mode_PWRCOACHEXX01</v>
       </c>
       <c r="AQ37" t="str">
-        <f>C37&amp;"*"</f>
+        <f t="shared" ref="AQ37:AQ70" si="5">C37&amp;"*"</f>
         <v>PWRCOACHEXX01*</v>
       </c>
       <c r="AR37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS37">
@@ -5551,7 +5466,7 @@
     </row>
     <row r="38" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D38">
         <v>0.9</v>
@@ -5662,19 +5577,19 @@
         <v>0.9</v>
       </c>
       <c r="AN38" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOADEUXX01</v>
+      </c>
+      <c r="AP38" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOADEUXX01</v>
+      </c>
+      <c r="AQ38" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOADEUXX01*</v>
+      </c>
+      <c r="AR38" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOADEUXX01</v>
-      </c>
-      <c r="AP38" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOADEUXX01</v>
-      </c>
-      <c r="AQ38" t="str">
-        <f>C38&amp;"*"</f>
-        <v>PWRCOADEUXX01*</v>
-      </c>
-      <c r="AR38" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS38">
@@ -5686,7 +5601,7 @@
     </row>
     <row r="39" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C39" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D39">
         <v>0.9</v>
@@ -5797,19 +5712,19 @@
         <v>0.9</v>
       </c>
       <c r="AN39" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOAESPXX01</v>
+      </c>
+      <c r="AP39" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOAESPXX01</v>
+      </c>
+      <c r="AQ39" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOAESPXX01*</v>
+      </c>
+      <c r="AR39" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOAESPXX01</v>
-      </c>
-      <c r="AP39" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOAESPXX01</v>
-      </c>
-      <c r="AQ39" t="str">
-        <f>C39&amp;"*"</f>
-        <v>PWRCOAESPXX01*</v>
-      </c>
-      <c r="AR39" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS39">
@@ -5821,7 +5736,7 @@
     </row>
     <row r="40" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C40" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D40">
         <v>0.9</v>
@@ -5932,19 +5847,19 @@
         <v>0.9</v>
       </c>
       <c r="AN40" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOAFRAXX01</v>
+      </c>
+      <c r="AP40" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOAFRAXX01</v>
+      </c>
+      <c r="AQ40" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOAFRAXX01*</v>
+      </c>
+      <c r="AR40" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOAFRAXX01</v>
-      </c>
-      <c r="AP40" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOAFRAXX01</v>
-      </c>
-      <c r="AQ40" t="str">
-        <f>C40&amp;"*"</f>
-        <v>PWRCOAFRAXX01*</v>
-      </c>
-      <c r="AR40" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS40">
@@ -5956,7 +5871,7 @@
     </row>
     <row r="41" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C41" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D41">
         <v>0.9</v>
@@ -6067,19 +5982,19 @@
         <v>0.9</v>
       </c>
       <c r="AN41" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOAITAXX01</v>
+      </c>
+      <c r="AP41" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOAITAXX01</v>
+      </c>
+      <c r="AQ41" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOAITAXX01*</v>
+      </c>
+      <c r="AR41" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOAITAXX01</v>
-      </c>
-      <c r="AP41" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOAITAXX01</v>
-      </c>
-      <c r="AQ41" t="str">
-        <f>C41&amp;"*"</f>
-        <v>PWRCOAITAXX01*</v>
-      </c>
-      <c r="AR41" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS41">
@@ -6091,7 +6006,7 @@
     </row>
     <row r="42" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C42" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D42">
         <v>0.9</v>
@@ -6202,19 +6117,19 @@
         <v>0.9</v>
       </c>
       <c r="AN42" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOALUXXX01</v>
+      </c>
+      <c r="AP42" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOALUXXX01</v>
+      </c>
+      <c r="AQ42" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOALUXXX01*</v>
+      </c>
+      <c r="AR42" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOALUXXX01</v>
-      </c>
-      <c r="AP42" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOALUXXX01</v>
-      </c>
-      <c r="AQ42" t="str">
-        <f>C42&amp;"*"</f>
-        <v>PWRCOALUXXX01*</v>
-      </c>
-      <c r="AR42" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS42">
@@ -6226,7 +6141,7 @@
     </row>
     <row r="43" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D43">
         <v>0.9</v>
@@ -6337,19 +6252,19 @@
         <v>0.9</v>
       </c>
       <c r="AN43" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOANLDXX01</v>
+      </c>
+      <c r="AP43" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOANLDXX01</v>
+      </c>
+      <c r="AQ43" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOANLDXX01*</v>
+      </c>
+      <c r="AR43" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOANLDXX01</v>
-      </c>
-      <c r="AP43" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOANLDXX01</v>
-      </c>
-      <c r="AQ43" t="str">
-        <f>C43&amp;"*"</f>
-        <v>PWRCOANLDXX01*</v>
-      </c>
-      <c r="AR43" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS43">
@@ -6361,7 +6276,7 @@
     </row>
     <row r="44" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C44" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D44">
         <v>0.9</v>
@@ -6472,19 +6387,19 @@
         <v>0.9</v>
       </c>
       <c r="AN44" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOAPRTXX01</v>
+      </c>
+      <c r="AP44" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOAPRTXX01</v>
+      </c>
+      <c r="AQ44" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOAPRTXX01*</v>
+      </c>
+      <c r="AR44" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOAPRTXX01</v>
-      </c>
-      <c r="AP44" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOAPRTXX01</v>
-      </c>
-      <c r="AQ44" t="str">
-        <f>C44&amp;"*"</f>
-        <v>PWRCOAPRTXX01*</v>
-      </c>
-      <c r="AR44" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS44">
@@ -6496,7 +6411,7 @@
     </row>
     <row r="45" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C45" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D45">
         <v>0.8</v>
@@ -6607,19 +6522,19 @@
         <v>0.8</v>
       </c>
       <c r="AN45" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGAUTXX01</v>
+      </c>
+      <c r="AP45" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGAUTXX01</v>
+      </c>
+      <c r="AQ45" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGAUTXX01*</v>
+      </c>
+      <c r="AR45" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGAUTXX01</v>
-      </c>
-      <c r="AP45" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGAUTXX01</v>
-      </c>
-      <c r="AQ45" t="str">
-        <f>C45&amp;"*"</f>
-        <v>PWRCOGAUTXX01*</v>
-      </c>
-      <c r="AR45" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS45">
@@ -6631,7 +6546,7 @@
     </row>
     <row r="46" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C46" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D46">
         <v>0.8</v>
@@ -6742,19 +6657,19 @@
         <v>0.8</v>
       </c>
       <c r="AN46" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGBELXX01</v>
+      </c>
+      <c r="AP46" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGBELXX01</v>
+      </c>
+      <c r="AQ46" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGBELXX01*</v>
+      </c>
+      <c r="AR46" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGBELXX01</v>
-      </c>
-      <c r="AP46" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGBELXX01</v>
-      </c>
-      <c r="AQ46" t="str">
-        <f>C46&amp;"*"</f>
-        <v>PWRCOGBELXX01*</v>
-      </c>
-      <c r="AR46" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS46">
@@ -6766,7 +6681,7 @@
     </row>
     <row r="47" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C47" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D47">
         <v>0.8</v>
@@ -6877,19 +6792,19 @@
         <v>0.8</v>
       </c>
       <c r="AN47" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGCHEXX01</v>
+      </c>
+      <c r="AP47" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGCHEXX01</v>
+      </c>
+      <c r="AQ47" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGCHEXX01*</v>
+      </c>
+      <c r="AR47" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGCHEXX01</v>
-      </c>
-      <c r="AP47" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGCHEXX01</v>
-      </c>
-      <c r="AQ47" t="str">
-        <f>C47&amp;"*"</f>
-        <v>PWRCOGCHEXX01*</v>
-      </c>
-      <c r="AR47" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS47">
@@ -6901,7 +6816,7 @@
     </row>
     <row r="48" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C48" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D48">
         <v>0.8</v>
@@ -7012,19 +6927,19 @@
         <v>0.8</v>
       </c>
       <c r="AN48" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGDEUXX01</v>
+      </c>
+      <c r="AP48" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGDEUXX01</v>
+      </c>
+      <c r="AQ48" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGDEUXX01*</v>
+      </c>
+      <c r="AR48" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGDEUXX01</v>
-      </c>
-      <c r="AP48" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGDEUXX01</v>
-      </c>
-      <c r="AQ48" t="str">
-        <f>C48&amp;"*"</f>
-        <v>PWRCOGDEUXX01*</v>
-      </c>
-      <c r="AR48" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS48">
@@ -7036,7 +6951,7 @@
     </row>
     <row r="49" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C49" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D49">
         <v>0.8</v>
@@ -7147,19 +7062,19 @@
         <v>0.8</v>
       </c>
       <c r="AN49" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGESPXX01</v>
+      </c>
+      <c r="AP49" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGESPXX01</v>
+      </c>
+      <c r="AQ49" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGESPXX01*</v>
+      </c>
+      <c r="AR49" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGESPXX01</v>
-      </c>
-      <c r="AP49" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGESPXX01</v>
-      </c>
-      <c r="AQ49" t="str">
-        <f>C49&amp;"*"</f>
-        <v>PWRCOGESPXX01*</v>
-      </c>
-      <c r="AR49" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS49">
@@ -7171,7 +7086,7 @@
     </row>
     <row r="50" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C50" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D50">
         <v>0.8</v>
@@ -7282,19 +7197,19 @@
         <v>0.8</v>
       </c>
       <c r="AN50" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGFRAXX01</v>
+      </c>
+      <c r="AP50" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGFRAXX01</v>
+      </c>
+      <c r="AQ50" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGFRAXX01*</v>
+      </c>
+      <c r="AR50" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGFRAXX01</v>
-      </c>
-      <c r="AP50" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGFRAXX01</v>
-      </c>
-      <c r="AQ50" t="str">
-        <f>C50&amp;"*"</f>
-        <v>PWRCOGFRAXX01*</v>
-      </c>
-      <c r="AR50" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS50">
@@ -7306,7 +7221,7 @@
     </row>
     <row r="51" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C51" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D51">
         <v>0.8</v>
@@ -7417,19 +7332,19 @@
         <v>0.8</v>
       </c>
       <c r="AN51" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGITAXX01</v>
+      </c>
+      <c r="AP51" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGITAXX01</v>
+      </c>
+      <c r="AQ51" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGITAXX01*</v>
+      </c>
+      <c r="AR51" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGITAXX01</v>
-      </c>
-      <c r="AP51" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGITAXX01</v>
-      </c>
-      <c r="AQ51" t="str">
-        <f>C51&amp;"*"</f>
-        <v>PWRCOGITAXX01*</v>
-      </c>
-      <c r="AR51" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS51">
@@ -7441,7 +7356,7 @@
     </row>
     <row r="52" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C52" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D52">
         <v>0.8</v>
@@ -7552,19 +7467,19 @@
         <v>0.8</v>
       </c>
       <c r="AN52" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGLUXXX01</v>
+      </c>
+      <c r="AP52" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGLUXXX01</v>
+      </c>
+      <c r="AQ52" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGLUXXX01*</v>
+      </c>
+      <c r="AR52" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGLUXXX01</v>
-      </c>
-      <c r="AP52" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGLUXXX01</v>
-      </c>
-      <c r="AQ52" t="str">
-        <f>C52&amp;"*"</f>
-        <v>PWRCOGLUXXX01*</v>
-      </c>
-      <c r="AR52" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS52">
@@ -7576,7 +7491,7 @@
     </row>
     <row r="53" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C53" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D53">
         <v>0.8</v>
@@ -7687,19 +7602,19 @@
         <v>0.8</v>
       </c>
       <c r="AN53" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGNLDXX01</v>
+      </c>
+      <c r="AP53" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGNLDXX01</v>
+      </c>
+      <c r="AQ53" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGNLDXX01*</v>
+      </c>
+      <c r="AR53" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGNLDXX01</v>
-      </c>
-      <c r="AP53" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGNLDXX01</v>
-      </c>
-      <c r="AQ53" t="str">
-        <f>C53&amp;"*"</f>
-        <v>PWRCOGNLDXX01*</v>
-      </c>
-      <c r="AR53" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS53">
@@ -7711,7 +7626,7 @@
     </row>
     <row r="54" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C54" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D54">
         <v>0.8</v>
@@ -7822,19 +7737,19 @@
         <v>0.8</v>
       </c>
       <c r="AN54" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWRCOGPRTXX01</v>
+      </c>
+      <c r="AP54" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWRCOGPRTXX01</v>
+      </c>
+      <c r="AQ54" t="str">
+        <f t="shared" si="5"/>
+        <v>PWRCOGPRTXX01*</v>
+      </c>
+      <c r="AR54" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWRCOGPRTXX01</v>
-      </c>
-      <c r="AP54" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWRCOGPRTXX01</v>
-      </c>
-      <c r="AQ54" t="str">
-        <f>C54&amp;"*"</f>
-        <v>PWRCOGPRTXX01*</v>
-      </c>
-      <c r="AR54" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS54">
@@ -7846,7 +7761,7 @@
     </row>
     <row r="55" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C55" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D55">
         <v>0.9</v>
@@ -7957,19 +7872,19 @@
         <v>0.9</v>
       </c>
       <c r="AN55" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGAUTXX00</v>
+      </c>
+      <c r="AP55" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGAUTXX00</v>
+      </c>
+      <c r="AQ55" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGAUTXX00*</v>
+      </c>
+      <c r="AR55" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGAUTXX00</v>
-      </c>
-      <c r="AP55" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGAUTXX00</v>
-      </c>
-      <c r="AQ55" t="str">
-        <f>C55&amp;"*"</f>
-        <v>PWROCGAUTXX00*</v>
-      </c>
-      <c r="AR55" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS55">
@@ -7981,7 +7896,7 @@
     </row>
     <row r="56" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C56" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D56">
         <v>0.9</v>
@@ -8092,19 +8007,19 @@
         <v>0.9</v>
       </c>
       <c r="AN56" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGAUTXX01</v>
+      </c>
+      <c r="AP56" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGAUTXX01</v>
+      </c>
+      <c r="AQ56" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGAUTXX01*</v>
+      </c>
+      <c r="AR56" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGAUTXX01</v>
-      </c>
-      <c r="AP56" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGAUTXX01</v>
-      </c>
-      <c r="AQ56" t="str">
-        <f>C56&amp;"*"</f>
-        <v>PWROCGAUTXX01*</v>
-      </c>
-      <c r="AR56" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS56">
@@ -8116,7 +8031,7 @@
     </row>
     <row r="57" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D57">
         <v>0.9</v>
@@ -8227,19 +8142,19 @@
         <v>0.9</v>
       </c>
       <c r="AN57" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGBELXX00</v>
+      </c>
+      <c r="AP57" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGBELXX00</v>
+      </c>
+      <c r="AQ57" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGBELXX00*</v>
+      </c>
+      <c r="AR57" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGBELXX00</v>
-      </c>
-      <c r="AP57" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGBELXX00</v>
-      </c>
-      <c r="AQ57" t="str">
-        <f>C57&amp;"*"</f>
-        <v>PWROCGBELXX00*</v>
-      </c>
-      <c r="AR57" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS57">
@@ -8251,7 +8166,7 @@
     </row>
     <row r="58" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D58">
         <v>0.9</v>
@@ -8362,19 +8277,19 @@
         <v>0.9</v>
       </c>
       <c r="AN58" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGBELXX01</v>
+      </c>
+      <c r="AP58" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGBELXX01</v>
+      </c>
+      <c r="AQ58" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGBELXX01*</v>
+      </c>
+      <c r="AR58" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGBELXX01</v>
-      </c>
-      <c r="AP58" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGBELXX01</v>
-      </c>
-      <c r="AQ58" t="str">
-        <f>C58&amp;"*"</f>
-        <v>PWROCGBELXX01*</v>
-      </c>
-      <c r="AR58" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS58">
@@ -8386,7 +8301,7 @@
     </row>
     <row r="59" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C59" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D59">
         <v>0.9</v>
@@ -8497,19 +8412,19 @@
         <v>0.9</v>
       </c>
       <c r="AN59" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGCHEXX00</v>
+      </c>
+      <c r="AP59" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGCHEXX00</v>
+      </c>
+      <c r="AQ59" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGCHEXX00*</v>
+      </c>
+      <c r="AR59" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGCHEXX00</v>
-      </c>
-      <c r="AP59" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGCHEXX00</v>
-      </c>
-      <c r="AQ59" t="str">
-        <f>C59&amp;"*"</f>
-        <v>PWROCGCHEXX00*</v>
-      </c>
-      <c r="AR59" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS59">
@@ -8521,7 +8436,7 @@
     </row>
     <row r="60" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C60" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D60">
         <v>0.9</v>
@@ -8632,19 +8547,19 @@
         <v>0.9</v>
       </c>
       <c r="AN60" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGCHEXX01</v>
+      </c>
+      <c r="AP60" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGCHEXX01</v>
+      </c>
+      <c r="AQ60" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGCHEXX01*</v>
+      </c>
+      <c r="AR60" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGCHEXX01</v>
-      </c>
-      <c r="AP60" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGCHEXX01</v>
-      </c>
-      <c r="AQ60" t="str">
-        <f>C60&amp;"*"</f>
-        <v>PWROCGCHEXX01*</v>
-      </c>
-      <c r="AR60" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS60">
@@ -8656,7 +8571,7 @@
     </row>
     <row r="61" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C61" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D61">
         <v>0.9</v>
@@ -8767,19 +8682,19 @@
         <v>0.9</v>
       </c>
       <c r="AN61" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGDEUXX00</v>
+      </c>
+      <c r="AP61" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGDEUXX00</v>
+      </c>
+      <c r="AQ61" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGDEUXX00*</v>
+      </c>
+      <c r="AR61" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGDEUXX00</v>
-      </c>
-      <c r="AP61" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGDEUXX00</v>
-      </c>
-      <c r="AQ61" t="str">
-        <f>C61&amp;"*"</f>
-        <v>PWROCGDEUXX00*</v>
-      </c>
-      <c r="AR61" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS61">
@@ -8791,7 +8706,7 @@
     </row>
     <row r="62" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C62" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D62">
         <v>0.9</v>
@@ -8902,19 +8817,19 @@
         <v>0.9</v>
       </c>
       <c r="AN62" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGDEUXX01</v>
+      </c>
+      <c r="AP62" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGDEUXX01</v>
+      </c>
+      <c r="AQ62" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGDEUXX01*</v>
+      </c>
+      <c r="AR62" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGDEUXX01</v>
-      </c>
-      <c r="AP62" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGDEUXX01</v>
-      </c>
-      <c r="AQ62" t="str">
-        <f>C62&amp;"*"</f>
-        <v>PWROCGDEUXX01*</v>
-      </c>
-      <c r="AR62" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS62">
@@ -8926,7 +8841,7 @@
     </row>
     <row r="63" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C63" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D63">
         <v>0.9</v>
@@ -9037,19 +8952,19 @@
         <v>0.9</v>
       </c>
       <c r="AN63" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGESPXX00</v>
+      </c>
+      <c r="AP63" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGESPXX00</v>
+      </c>
+      <c r="AQ63" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGESPXX00*</v>
+      </c>
+      <c r="AR63" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGESPXX00</v>
-      </c>
-      <c r="AP63" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGESPXX00</v>
-      </c>
-      <c r="AQ63" t="str">
-        <f>C63&amp;"*"</f>
-        <v>PWROCGESPXX00*</v>
-      </c>
-      <c r="AR63" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS63">
@@ -9061,7 +8976,7 @@
     </row>
     <row r="64" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C64" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D64">
         <v>0.9</v>
@@ -9172,19 +9087,19 @@
         <v>0.9</v>
       </c>
       <c r="AN64" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGESPXX01</v>
+      </c>
+      <c r="AP64" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGESPXX01</v>
+      </c>
+      <c r="AQ64" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGESPXX01*</v>
+      </c>
+      <c r="AR64" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGESPXX01</v>
-      </c>
-      <c r="AP64" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGESPXX01</v>
-      </c>
-      <c r="AQ64" t="str">
-        <f>C64&amp;"*"</f>
-        <v>PWROCGESPXX01*</v>
-      </c>
-      <c r="AR64" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS64">
@@ -9196,7 +9111,7 @@
     </row>
     <row r="65" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C65" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D65">
         <v>0.9</v>
@@ -9307,19 +9222,19 @@
         <v>0.9</v>
       </c>
       <c r="AN65" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGFRAXX00</v>
+      </c>
+      <c r="AP65" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGFRAXX00</v>
+      </c>
+      <c r="AQ65" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGFRAXX00*</v>
+      </c>
+      <c r="AR65" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGFRAXX00</v>
-      </c>
-      <c r="AP65" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGFRAXX00</v>
-      </c>
-      <c r="AQ65" t="str">
-        <f>C65&amp;"*"</f>
-        <v>PWROCGFRAXX00*</v>
-      </c>
-      <c r="AR65" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS65">
@@ -9331,7 +9246,7 @@
     </row>
     <row r="66" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C66" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D66">
         <v>0.9</v>
@@ -9442,19 +9357,19 @@
         <v>0.9</v>
       </c>
       <c r="AN66" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGFRAXX01</v>
+      </c>
+      <c r="AP66" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGFRAXX01</v>
+      </c>
+      <c r="AQ66" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGFRAXX01*</v>
+      </c>
+      <c r="AR66" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGFRAXX01</v>
-      </c>
-      <c r="AP66" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGFRAXX01</v>
-      </c>
-      <c r="AQ66" t="str">
-        <f>C66&amp;"*"</f>
-        <v>PWROCGFRAXX01*</v>
-      </c>
-      <c r="AR66" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS66">
@@ -9466,7 +9381,7 @@
     </row>
     <row r="67" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C67" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D67">
         <v>0.9</v>
@@ -9577,19 +9492,19 @@
         <v>0.9</v>
       </c>
       <c r="AN67" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGITAXX00</v>
+      </c>
+      <c r="AP67" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGITAXX00</v>
+      </c>
+      <c r="AQ67" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGITAXX00*</v>
+      </c>
+      <c r="AR67" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGITAXX00</v>
-      </c>
-      <c r="AP67" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGITAXX00</v>
-      </c>
-      <c r="AQ67" t="str">
-        <f>C67&amp;"*"</f>
-        <v>PWROCGITAXX00*</v>
-      </c>
-      <c r="AR67" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS67">
@@ -9601,7 +9516,7 @@
     </row>
     <row r="68" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C68" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D68">
         <v>0.9</v>
@@ -9712,19 +9627,19 @@
         <v>0.9</v>
       </c>
       <c r="AN68" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGITAXX01</v>
+      </c>
+      <c r="AP68" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGITAXX01</v>
+      </c>
+      <c r="AQ68" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGITAXX01*</v>
+      </c>
+      <c r="AR68" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGITAXX01</v>
-      </c>
-      <c r="AP68" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGITAXX01</v>
-      </c>
-      <c r="AQ68" t="str">
-        <f>C68&amp;"*"</f>
-        <v>PWROCGITAXX01*</v>
-      </c>
-      <c r="AR68" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS68">
@@ -9736,7 +9651,7 @@
     </row>
     <row r="69" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C69" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D69">
         <v>0.9</v>
@@ -9847,19 +9762,19 @@
         <v>0.9</v>
       </c>
       <c r="AN69" t="str">
+        <f t="shared" si="4"/>
+        <v>op mode_PWROCGLUXXX00</v>
+      </c>
+      <c r="AP69" t="str">
+        <f t="shared" si="2"/>
+        <v>op mode_PWROCGLUXXX00</v>
+      </c>
+      <c r="AQ69" t="str">
+        <f t="shared" si="5"/>
+        <v>PWROCGLUXXX00*</v>
+      </c>
+      <c r="AR69" s="1">
         <f t="shared" si="3"/>
-        <v>op mode_PWROCGLUXXX00</v>
-      </c>
-      <c r="AP69" t="str">
-        <f t="shared" si="1"/>
-        <v>op mode_PWROCGLUXXX00</v>
-      </c>
-      <c r="AQ69" t="str">
-        <f>C69&amp;"*"</f>
-        <v>PWROCGLUXXX00*</v>
-      </c>
-      <c r="AR69" s="1">
-        <f t="shared" si="2"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS69">
@@ -9871,7 +9786,7 @@
     </row>
     <row r="70" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C70" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D70">
         <v>0.9</v>
@@ -9982,19 +9897,19 @@
         <v>0.9</v>
       </c>
       <c r="AN70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>op mode_PWROCGLUXXX01</v>
       </c>
       <c r="AP70" t="str">
-        <f t="shared" ref="AP70" si="4">AN70</f>
+        <f t="shared" ref="AP70" si="6">AN70</f>
         <v>op mode_PWROCGLUXXX01</v>
       </c>
       <c r="AQ70" t="str">
-        <f>C70&amp;"*"</f>
+        <f t="shared" si="5"/>
         <v>PWROCGLUXXX01*</v>
       </c>
       <c r="AR70" s="1">
-        <f t="shared" ref="AR70:AR114" si="5">-1/31.536</f>
+        <f t="shared" ref="AR70:AR114" si="7">-1/31.536</f>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS70">
@@ -10006,7 +9921,7 @@
     </row>
     <row r="71" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C71" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D71">
         <v>0.9</v>
@@ -10117,19 +10032,19 @@
         <v>0.9</v>
       </c>
       <c r="AN71" t="str">
-        <f t="shared" ref="AN71:AN114" si="6">"op mode_"&amp;LEFT(AQ71,LEN(AQ71)-1)</f>
+        <f t="shared" ref="AN71:AN114" si="8">"op mode_"&amp;LEFT(AQ71,LEN(AQ71)-1)</f>
         <v>op mode_PWROCGNLDXX00</v>
       </c>
       <c r="AP71" t="str">
-        <f t="shared" ref="AP71:AP114" si="7">AN71</f>
+        <f t="shared" ref="AP71:AP114" si="9">AN71</f>
         <v>op mode_PWROCGNLDXX00</v>
       </c>
       <c r="AQ71" t="str">
-        <f t="shared" ref="AQ71:AQ114" si="8">C71&amp;"*"</f>
+        <f t="shared" ref="AQ71:AQ114" si="10">C71&amp;"*"</f>
         <v>PWROCGNLDXX00*</v>
       </c>
       <c r="AR71" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS71">
@@ -10141,7 +10056,7 @@
     </row>
     <row r="72" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C72" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D72">
         <v>0.9</v>
@@ -10252,19 +10167,19 @@
         <v>0.9</v>
       </c>
       <c r="AN72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROCGNLDXX01</v>
       </c>
       <c r="AP72" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROCGNLDXX01</v>
+      </c>
+      <c r="AQ72" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROCGNLDXX01*</v>
+      </c>
+      <c r="AR72" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROCGNLDXX01</v>
-      </c>
-      <c r="AQ72" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROCGNLDXX01*</v>
-      </c>
-      <c r="AR72" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS72">
@@ -10276,7 +10191,7 @@
     </row>
     <row r="73" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C73" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D73">
         <v>0.9</v>
@@ -10387,19 +10302,19 @@
         <v>0.9</v>
       </c>
       <c r="AN73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROCGPRTXX00</v>
       </c>
       <c r="AP73" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROCGPRTXX00</v>
+      </c>
+      <c r="AQ73" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROCGPRTXX00*</v>
+      </c>
+      <c r="AR73" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROCGPRTXX00</v>
-      </c>
-      <c r="AQ73" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROCGPRTXX00*</v>
-      </c>
-      <c r="AR73" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS73">
@@ -10411,7 +10326,7 @@
     </row>
     <row r="74" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C74" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D74">
         <v>0.9</v>
@@ -10522,19 +10437,19 @@
         <v>0.9</v>
       </c>
       <c r="AN74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROCGPRTXX01</v>
       </c>
       <c r="AP74" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROCGPRTXX01</v>
+      </c>
+      <c r="AQ74" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROCGPRTXX01*</v>
+      </c>
+      <c r="AR74" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROCGPRTXX01</v>
-      </c>
-      <c r="AQ74" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROCGPRTXX01*</v>
-      </c>
-      <c r="AR74" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS74">
@@ -10546,7 +10461,7 @@
     </row>
     <row r="75" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C75" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D75">
         <v>0.8</v>
@@ -10657,19 +10572,19 @@
         <v>0.8</v>
       </c>
       <c r="AN75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILAUTXX01</v>
       </c>
       <c r="AP75" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILAUTXX01</v>
+      </c>
+      <c r="AQ75" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILAUTXX01*</v>
+      </c>
+      <c r="AR75" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILAUTXX01</v>
-      </c>
-      <c r="AQ75" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILAUTXX01*</v>
-      </c>
-      <c r="AR75" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS75">
@@ -10681,7 +10596,7 @@
     </row>
     <row r="76" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C76" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D76">
         <v>0.8</v>
@@ -10792,19 +10707,19 @@
         <v>0.8</v>
       </c>
       <c r="AN76" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILBELXX01</v>
       </c>
       <c r="AP76" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILBELXX01</v>
+      </c>
+      <c r="AQ76" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILBELXX01*</v>
+      </c>
+      <c r="AR76" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILBELXX01</v>
-      </c>
-      <c r="AQ76" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILBELXX01*</v>
-      </c>
-      <c r="AR76" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS76">
@@ -10816,7 +10731,7 @@
     </row>
     <row r="77" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C77" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D77">
         <v>0.8</v>
@@ -10927,19 +10842,19 @@
         <v>0.8</v>
       </c>
       <c r="AN77" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILCHEXX01</v>
       </c>
       <c r="AP77" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILCHEXX01</v>
+      </c>
+      <c r="AQ77" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILCHEXX01*</v>
+      </c>
+      <c r="AR77" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILCHEXX01</v>
-      </c>
-      <c r="AQ77" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILCHEXX01*</v>
-      </c>
-      <c r="AR77" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS77">
@@ -10951,7 +10866,7 @@
     </row>
     <row r="78" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C78" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D78">
         <v>0.8</v>
@@ -11062,19 +10977,19 @@
         <v>0.8</v>
       </c>
       <c r="AN78" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILDEUXX01</v>
       </c>
       <c r="AP78" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILDEUXX01</v>
+      </c>
+      <c r="AQ78" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILDEUXX01*</v>
+      </c>
+      <c r="AR78" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILDEUXX01</v>
-      </c>
-      <c r="AQ78" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILDEUXX01*</v>
-      </c>
-      <c r="AR78" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS78">
@@ -11086,7 +11001,7 @@
     </row>
     <row r="79" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C79" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D79">
         <v>0.8</v>
@@ -11197,19 +11112,19 @@
         <v>0.8</v>
       </c>
       <c r="AN79" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILESPXX01</v>
       </c>
       <c r="AP79" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILESPXX01</v>
+      </c>
+      <c r="AQ79" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILESPXX01*</v>
+      </c>
+      <c r="AR79" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILESPXX01</v>
-      </c>
-      <c r="AQ79" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILESPXX01*</v>
-      </c>
-      <c r="AR79" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS79">
@@ -11221,7 +11136,7 @@
     </row>
     <row r="80" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C80" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D80">
         <v>0.8</v>
@@ -11332,19 +11247,19 @@
         <v>0.8</v>
       </c>
       <c r="AN80" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILFRAXX01</v>
       </c>
       <c r="AP80" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILFRAXX01</v>
+      </c>
+      <c r="AQ80" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILFRAXX01*</v>
+      </c>
+      <c r="AR80" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILFRAXX01</v>
-      </c>
-      <c r="AQ80" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILFRAXX01*</v>
-      </c>
-      <c r="AR80" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS80">
@@ -11356,7 +11271,7 @@
     </row>
     <row r="81" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C81" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D81">
         <v>0.8</v>
@@ -11467,19 +11382,19 @@
         <v>0.8</v>
       </c>
       <c r="AN81" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILITAXX01</v>
       </c>
       <c r="AP81" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILITAXX01</v>
+      </c>
+      <c r="AQ81" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILITAXX01*</v>
+      </c>
+      <c r="AR81" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILITAXX01</v>
-      </c>
-      <c r="AQ81" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILITAXX01*</v>
-      </c>
-      <c r="AR81" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS81">
@@ -11491,7 +11406,7 @@
     </row>
     <row r="82" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C82" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D82">
         <v>0.8</v>
@@ -11602,19 +11517,19 @@
         <v>0.8</v>
       </c>
       <c r="AN82" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILLUXXX01</v>
       </c>
       <c r="AP82" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILLUXXX01</v>
+      </c>
+      <c r="AQ82" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILLUXXX01*</v>
+      </c>
+      <c r="AR82" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILLUXXX01</v>
-      </c>
-      <c r="AQ82" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILLUXXX01*</v>
-      </c>
-      <c r="AR82" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS82">
@@ -11626,7 +11541,7 @@
     </row>
     <row r="83" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C83" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D83">
         <v>0.8</v>
@@ -11737,19 +11652,19 @@
         <v>0.8</v>
       </c>
       <c r="AN83" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILNLDXX01</v>
       </c>
       <c r="AP83" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILNLDXX01</v>
+      </c>
+      <c r="AQ83" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILNLDXX01*</v>
+      </c>
+      <c r="AR83" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILNLDXX01</v>
-      </c>
-      <c r="AQ83" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILNLDXX01*</v>
-      </c>
-      <c r="AR83" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS83">
@@ -11761,7 +11676,7 @@
     </row>
     <row r="84" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C84" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D84">
         <v>0.8</v>
@@ -11872,19 +11787,19 @@
         <v>0.8</v>
       </c>
       <c r="AN84" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROILPRTXX01</v>
       </c>
       <c r="AP84" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROILPRTXX01</v>
+      </c>
+      <c r="AQ84" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROILPRTXX01*</v>
+      </c>
+      <c r="AR84" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROILPRTXX01</v>
-      </c>
-      <c r="AQ84" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROILPRTXX01*</v>
-      </c>
-      <c r="AR84" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS84">
@@ -11896,7 +11811,7 @@
     </row>
     <row r="85" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C85" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D85">
         <v>0.8</v>
@@ -12007,19 +11922,19 @@
         <v>0.8</v>
       </c>
       <c r="AN85" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHAUTXX01</v>
       </c>
       <c r="AP85" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHAUTXX01</v>
+      </c>
+      <c r="AQ85" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHAUTXX01*</v>
+      </c>
+      <c r="AR85" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHAUTXX01</v>
-      </c>
-      <c r="AQ85" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHAUTXX01*</v>
-      </c>
-      <c r="AR85" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS85">
@@ -12031,7 +11946,7 @@
     </row>
     <row r="86" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C86" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D86">
         <v>0.8</v>
@@ -12142,19 +12057,19 @@
         <v>0.8</v>
       </c>
       <c r="AN86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHBELXX01</v>
       </c>
       <c r="AP86" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHBELXX01</v>
+      </c>
+      <c r="AQ86" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHBELXX01*</v>
+      </c>
+      <c r="AR86" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHBELXX01</v>
-      </c>
-      <c r="AQ86" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHBELXX01*</v>
-      </c>
-      <c r="AR86" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS86">
@@ -12166,7 +12081,7 @@
     </row>
     <row r="87" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C87" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D87">
         <v>0.8</v>
@@ -12277,19 +12192,19 @@
         <v>0.8</v>
       </c>
       <c r="AN87" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHCHEXX01</v>
       </c>
       <c r="AP87" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHCHEXX01</v>
+      </c>
+      <c r="AQ87" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHCHEXX01*</v>
+      </c>
+      <c r="AR87" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHCHEXX01</v>
-      </c>
-      <c r="AQ87" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHCHEXX01*</v>
-      </c>
-      <c r="AR87" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS87">
@@ -12301,7 +12216,7 @@
     </row>
     <row r="88" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C88" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D88">
         <v>0.8</v>
@@ -12412,19 +12327,19 @@
         <v>0.8</v>
       </c>
       <c r="AN88" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHDEUXX01</v>
       </c>
       <c r="AP88" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHDEUXX01</v>
+      </c>
+      <c r="AQ88" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHDEUXX01*</v>
+      </c>
+      <c r="AR88" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHDEUXX01</v>
-      </c>
-      <c r="AQ88" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHDEUXX01*</v>
-      </c>
-      <c r="AR88" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS88">
@@ -12436,7 +12351,7 @@
     </row>
     <row r="89" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C89" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D89">
         <v>0.8</v>
@@ -12547,19 +12462,19 @@
         <v>0.8</v>
       </c>
       <c r="AN89" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHESPXX01</v>
       </c>
       <c r="AP89" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHESPXX01</v>
+      </c>
+      <c r="AQ89" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHESPXX01*</v>
+      </c>
+      <c r="AR89" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHESPXX01</v>
-      </c>
-      <c r="AQ89" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHESPXX01*</v>
-      </c>
-      <c r="AR89" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS89">
@@ -12571,7 +12486,7 @@
     </row>
     <row r="90" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C90" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D90">
         <v>0.8</v>
@@ -12682,19 +12597,19 @@
         <v>0.8</v>
       </c>
       <c r="AN90" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHFRAXX01</v>
       </c>
       <c r="AP90" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHFRAXX01</v>
+      </c>
+      <c r="AQ90" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHFRAXX01*</v>
+      </c>
+      <c r="AR90" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHFRAXX01</v>
-      </c>
-      <c r="AQ90" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHFRAXX01*</v>
-      </c>
-      <c r="AR90" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS90">
@@ -12706,7 +12621,7 @@
     </row>
     <row r="91" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C91" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D91">
         <v>0.8</v>
@@ -12817,19 +12732,19 @@
         <v>0.8</v>
       </c>
       <c r="AN91" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHITAXX01</v>
       </c>
       <c r="AP91" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHITAXX01</v>
+      </c>
+      <c r="AQ91" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHITAXX01*</v>
+      </c>
+      <c r="AR91" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHITAXX01</v>
-      </c>
-      <c r="AQ91" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHITAXX01*</v>
-      </c>
-      <c r="AR91" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS91">
@@ -12841,7 +12756,7 @@
     </row>
     <row r="92" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C92" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D92">
         <v>0.8</v>
@@ -12952,19 +12867,19 @@
         <v>0.8</v>
       </c>
       <c r="AN92" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHLUXXX01</v>
       </c>
       <c r="AP92" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHLUXXX01</v>
+      </c>
+      <c r="AQ92" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHLUXXX01*</v>
+      </c>
+      <c r="AR92" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHLUXXX01</v>
-      </c>
-      <c r="AQ92" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHLUXXX01*</v>
-      </c>
-      <c r="AR92" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS92">
@@ -12976,7 +12891,7 @@
     </row>
     <row r="93" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C93" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D93">
         <v>0.8</v>
@@ -13087,19 +13002,19 @@
         <v>0.8</v>
       </c>
       <c r="AN93" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHNLDXX01</v>
       </c>
       <c r="AP93" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHNLDXX01</v>
+      </c>
+      <c r="AQ93" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHNLDXX01*</v>
+      </c>
+      <c r="AR93" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHNLDXX01</v>
-      </c>
-      <c r="AQ93" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHNLDXX01*</v>
-      </c>
-      <c r="AR93" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS93">
@@ -13111,7 +13026,7 @@
     </row>
     <row r="94" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C94" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D94">
         <v>0.8</v>
@@ -13222,19 +13137,19 @@
         <v>0.8</v>
       </c>
       <c r="AN94" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWROTHPRTXX01</v>
       </c>
       <c r="AP94" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWROTHPRTXX01</v>
+      </c>
+      <c r="AQ94" t="str">
+        <f t="shared" si="10"/>
+        <v>PWROTHPRTXX01*</v>
+      </c>
+      <c r="AR94" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWROTHPRTXX01</v>
-      </c>
-      <c r="AQ94" t="str">
-        <f t="shared" si="8"/>
-        <v>PWROTHPRTXX01*</v>
-      </c>
-      <c r="AR94" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS94">
@@ -13246,7 +13161,7 @@
     </row>
     <row r="95" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C95" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D95">
         <v>0.8</v>
@@ -13357,19 +13272,19 @@
         <v>0.8</v>
       </c>
       <c r="AN95" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETAUTXX01</v>
       </c>
       <c r="AP95" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETAUTXX01</v>
+      </c>
+      <c r="AQ95" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETAUTXX01*</v>
+      </c>
+      <c r="AR95" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETAUTXX01</v>
-      </c>
-      <c r="AQ95" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETAUTXX01*</v>
-      </c>
-      <c r="AR95" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS95">
@@ -13381,7 +13296,7 @@
     </row>
     <row r="96" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C96" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D96">
         <v>0.8</v>
@@ -13492,19 +13407,19 @@
         <v>0.8</v>
       </c>
       <c r="AN96" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETBELXX01</v>
       </c>
       <c r="AP96" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETBELXX01</v>
+      </c>
+      <c r="AQ96" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETBELXX01*</v>
+      </c>
+      <c r="AR96" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETBELXX01</v>
-      </c>
-      <c r="AQ96" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETBELXX01*</v>
-      </c>
-      <c r="AR96" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS96">
@@ -13516,7 +13431,7 @@
     </row>
     <row r="97" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C97" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D97">
         <v>0.8</v>
@@ -13627,19 +13542,19 @@
         <v>0.8</v>
       </c>
       <c r="AN97" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETCHEXX01</v>
       </c>
       <c r="AP97" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETCHEXX01</v>
+      </c>
+      <c r="AQ97" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETCHEXX01*</v>
+      </c>
+      <c r="AR97" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETCHEXX01</v>
-      </c>
-      <c r="AQ97" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETCHEXX01*</v>
-      </c>
-      <c r="AR97" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS97">
@@ -13651,7 +13566,7 @@
     </row>
     <row r="98" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C98" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D98">
         <v>0.8</v>
@@ -13762,19 +13677,19 @@
         <v>0.8</v>
       </c>
       <c r="AN98" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETDEUXX01</v>
       </c>
       <c r="AP98" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETDEUXX01</v>
+      </c>
+      <c r="AQ98" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETDEUXX01*</v>
+      </c>
+      <c r="AR98" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETDEUXX01</v>
-      </c>
-      <c r="AQ98" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETDEUXX01*</v>
-      </c>
-      <c r="AR98" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS98">
@@ -13786,7 +13701,7 @@
     </row>
     <row r="99" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C99" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D99">
         <v>0.8</v>
@@ -13897,19 +13812,19 @@
         <v>0.8</v>
       </c>
       <c r="AN99" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETESPXX01</v>
       </c>
       <c r="AP99" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETESPXX01</v>
+      </c>
+      <c r="AQ99" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETESPXX01*</v>
+      </c>
+      <c r="AR99" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETESPXX01</v>
-      </c>
-      <c r="AQ99" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETESPXX01*</v>
-      </c>
-      <c r="AR99" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS99">
@@ -13921,7 +13836,7 @@
     </row>
     <row r="100" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C100" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D100">
         <v>0.8</v>
@@ -14032,19 +13947,19 @@
         <v>0.8</v>
       </c>
       <c r="AN100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETFRAXX01</v>
       </c>
       <c r="AP100" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETFRAXX01</v>
+      </c>
+      <c r="AQ100" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETFRAXX01*</v>
+      </c>
+      <c r="AR100" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETFRAXX01</v>
-      </c>
-      <c r="AQ100" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETFRAXX01*</v>
-      </c>
-      <c r="AR100" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS100">
@@ -14056,7 +13971,7 @@
     </row>
     <row r="101" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C101" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D101">
         <v>0.8</v>
@@ -14167,19 +14082,19 @@
         <v>0.8</v>
       </c>
       <c r="AN101" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETITAXX01</v>
       </c>
       <c r="AP101" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETITAXX01</v>
+      </c>
+      <c r="AQ101" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETITAXX01*</v>
+      </c>
+      <c r="AR101" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETITAXX01</v>
-      </c>
-      <c r="AQ101" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETITAXX01*</v>
-      </c>
-      <c r="AR101" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS101">
@@ -14191,7 +14106,7 @@
     </row>
     <row r="102" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C102" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D102">
         <v>0.8</v>
@@ -14302,19 +14217,19 @@
         <v>0.8</v>
       </c>
       <c r="AN102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETLUXXX01</v>
       </c>
       <c r="AP102" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETLUXXX01</v>
+      </c>
+      <c r="AQ102" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETLUXXX01*</v>
+      </c>
+      <c r="AR102" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETLUXXX01</v>
-      </c>
-      <c r="AQ102" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETLUXXX01*</v>
-      </c>
-      <c r="AR102" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS102">
@@ -14326,7 +14241,7 @@
     </row>
     <row r="103" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C103" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D103">
         <v>0.8</v>
@@ -14437,19 +14352,19 @@
         <v>0.8</v>
       </c>
       <c r="AN103" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETNLDXX01</v>
       </c>
       <c r="AP103" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETNLDXX01</v>
+      </c>
+      <c r="AQ103" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETNLDXX01*</v>
+      </c>
+      <c r="AR103" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETNLDXX01</v>
-      </c>
-      <c r="AQ103" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETNLDXX01*</v>
-      </c>
-      <c r="AR103" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS103">
@@ -14461,7 +14376,7 @@
     </row>
     <row r="104" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C104" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D104">
         <v>0.8</v>
@@ -14572,19 +14487,19 @@
         <v>0.8</v>
       </c>
       <c r="AN104" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRPETPRTXX01</v>
       </c>
       <c r="AP104" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRPETPRTXX01</v>
+      </c>
+      <c r="AQ104" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRPETPRTXX01*</v>
+      </c>
+      <c r="AR104" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRPETPRTXX01</v>
-      </c>
-      <c r="AQ104" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRPETPRTXX01*</v>
-      </c>
-      <c r="AR104" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS104">
@@ -14596,7 +14511,7 @@
     </row>
     <row r="105" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C105" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D105">
         <v>0.9</v>
@@ -14707,19 +14622,19 @@
         <v>0.9</v>
       </c>
       <c r="AN105" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNAUTXX01</v>
       </c>
       <c r="AP105" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNAUTXX01</v>
+      </c>
+      <c r="AQ105" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNAUTXX01*</v>
+      </c>
+      <c r="AR105" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNAUTXX01</v>
-      </c>
-      <c r="AQ105" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNAUTXX01*</v>
-      </c>
-      <c r="AR105" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS105">
@@ -14731,7 +14646,7 @@
     </row>
     <row r="106" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C106" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D106">
         <v>0.9</v>
@@ -14842,19 +14757,19 @@
         <v>0.9</v>
       </c>
       <c r="AN106" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNBELXX01</v>
       </c>
       <c r="AP106" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNBELXX01</v>
+      </c>
+      <c r="AQ106" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNBELXX01*</v>
+      </c>
+      <c r="AR106" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNBELXX01</v>
-      </c>
-      <c r="AQ106" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNBELXX01*</v>
-      </c>
-      <c r="AR106" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS106">
@@ -14866,7 +14781,7 @@
     </row>
     <row r="107" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C107" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D107">
         <v>0.9</v>
@@ -14977,19 +14892,19 @@
         <v>0.9</v>
       </c>
       <c r="AN107" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNCHEXX01</v>
       </c>
       <c r="AP107" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNCHEXX01</v>
+      </c>
+      <c r="AQ107" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNCHEXX01*</v>
+      </c>
+      <c r="AR107" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNCHEXX01</v>
-      </c>
-      <c r="AQ107" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNCHEXX01*</v>
-      </c>
-      <c r="AR107" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS107">
@@ -15001,7 +14916,7 @@
     </row>
     <row r="108" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C108" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D108">
         <v>0.9</v>
@@ -15112,19 +15027,19 @@
         <v>0.9</v>
       </c>
       <c r="AN108" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNDEUXX01</v>
       </c>
       <c r="AP108" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNDEUXX01</v>
+      </c>
+      <c r="AQ108" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNDEUXX01*</v>
+      </c>
+      <c r="AR108" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNDEUXX01</v>
-      </c>
-      <c r="AQ108" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNDEUXX01*</v>
-      </c>
-      <c r="AR108" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS108">
@@ -15136,7 +15051,7 @@
     </row>
     <row r="109" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C109" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D109">
         <v>0.9</v>
@@ -15247,19 +15162,19 @@
         <v>0.9</v>
       </c>
       <c r="AN109" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNESPXX01</v>
       </c>
       <c r="AP109" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNESPXX01</v>
+      </c>
+      <c r="AQ109" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNESPXX01*</v>
+      </c>
+      <c r="AR109" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNESPXX01</v>
-      </c>
-      <c r="AQ109" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNESPXX01*</v>
-      </c>
-      <c r="AR109" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS109">
@@ -15271,7 +15186,7 @@
     </row>
     <row r="110" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C110" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D110">
         <v>0.9</v>
@@ -15382,19 +15297,19 @@
         <v>0.9</v>
       </c>
       <c r="AN110" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNFRAXX01</v>
       </c>
       <c r="AP110" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNFRAXX01</v>
+      </c>
+      <c r="AQ110" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNFRAXX01*</v>
+      </c>
+      <c r="AR110" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNFRAXX01</v>
-      </c>
-      <c r="AQ110" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNFRAXX01*</v>
-      </c>
-      <c r="AR110" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS110">
@@ -15406,7 +15321,7 @@
     </row>
     <row r="111" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C111" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D111">
         <v>0.9</v>
@@ -15517,19 +15432,19 @@
         <v>0.9</v>
       </c>
       <c r="AN111" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNITAXX01</v>
       </c>
       <c r="AP111" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNITAXX01</v>
+      </c>
+      <c r="AQ111" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNITAXX01*</v>
+      </c>
+      <c r="AR111" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNITAXX01</v>
-      </c>
-      <c r="AQ111" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNITAXX01*</v>
-      </c>
-      <c r="AR111" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS111">
@@ -15541,7 +15456,7 @@
     </row>
     <row r="112" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C112" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D112">
         <v>0.9</v>
@@ -15652,19 +15567,19 @@
         <v>0.9</v>
       </c>
       <c r="AN112" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNLUXXX01</v>
       </c>
       <c r="AP112" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNLUXXX01</v>
+      </c>
+      <c r="AQ112" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNLUXXX01*</v>
+      </c>
+      <c r="AR112" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNLUXXX01</v>
-      </c>
-      <c r="AQ112" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNLUXXX01*</v>
-      </c>
-      <c r="AR112" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS112">
@@ -15676,7 +15591,7 @@
     </row>
     <row r="113" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C113" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D113">
         <v>0.9</v>
@@ -15787,19 +15702,19 @@
         <v>0.9</v>
       </c>
       <c r="AN113" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNNLDXX01</v>
       </c>
       <c r="AP113" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNNLDXX01</v>
+      </c>
+      <c r="AQ113" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNNLDXX01*</v>
+      </c>
+      <c r="AR113" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNNLDXX01</v>
-      </c>
-      <c r="AQ113" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNNLDXX01*</v>
-      </c>
-      <c r="AR113" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS113">
@@ -15811,7 +15726,7 @@
     </row>
     <row r="114" spans="3:46" x14ac:dyDescent="0.5">
       <c r="C114" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D114">
         <v>0.9</v>
@@ -15922,19 +15837,19 @@
         <v>0.9</v>
       </c>
       <c r="AN114" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>op mode_PWRURNPRTXX01</v>
       </c>
       <c r="AP114" t="str">
+        <f t="shared" si="9"/>
+        <v>op mode_PWRURNPRTXX01</v>
+      </c>
+      <c r="AQ114" t="str">
+        <f t="shared" si="10"/>
+        <v>PWRURNPRTXX01*</v>
+      </c>
+      <c r="AR114" s="1">
         <f t="shared" si="7"/>
-        <v>op mode_PWRURNPRTXX01</v>
-      </c>
-      <c r="AQ114" t="str">
-        <f t="shared" si="8"/>
-        <v>PWRURNPRTXX01*</v>
-      </c>
-      <c r="AR114" s="1">
-        <f t="shared" si="5"/>
         <v>-3.1709791983764585E-2</v>
       </c>
       <c r="AS114">

</xml_diff>